<commit_message>
Filter Dropdown and Config Database
</commit_message>
<xml_diff>
--- a/static/excel/Database.xlsx
+++ b/static/excel/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narav\Downloads\maximo\WebConverter\maximo_project\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A1C18-026C-4A6D-AC08-0A415890A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E98E4C-385D-4F0D-87C6-98769B66C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SITE" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,10 @@
     <sheet name="WBS" sheetId="6" r:id="rId6"/>
     <sheet name="STATUS" sheetId="7" r:id="rId7"/>
     <sheet name="Site-PlantType" sheetId="8" r:id="rId8"/>
+    <sheet name="ChildSite" sheetId="9" r:id="rId9"/>
+    <sheet name="Site-ChildSite" sheetId="10" r:id="rId10"/>
+    <sheet name="PlantType-ActType" sheetId="11" r:id="rId11"/>
+    <sheet name="PlantType-WorkType" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="230">
   <si>
     <t>BLG0</t>
   </si>
@@ -535,13 +539,211 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>NPU</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำขนาดเล็กเขื่อนน้ำพุง</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนศรีนครินทร์</t>
+  </si>
+  <si>
+    <t>URD</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนอุบลรัตน์</t>
+  </si>
+  <si>
+    <t>BLG</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนบางลาง</t>
+  </si>
+  <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนขนาดเล็กบ้านสันติ</t>
+  </si>
+  <si>
+    <t>BMB</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนภูมิพล</t>
+  </si>
+  <si>
+    <t>CPY</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนเจ้าพระยา</t>
+  </si>
+  <si>
+    <t>KKM</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าเขื่อนกิ่วคอหมา</t>
+  </si>
+  <si>
+    <t>SKP</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังแสงอาทิตย์สันกำแพง</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังความร้อนใต้พิภพฝาง</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าดีเซลแม่ฮ่องสอน</t>
+  </si>
+  <si>
+    <t>PHB</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังแสงอาทิตย์ผาบ่อง</t>
+  </si>
+  <si>
+    <t>MNG</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนขนาดเล็กเขื่อนแม่งัดสมบูรณ์ชล</t>
+  </si>
+  <si>
+    <t>BKG</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำบ้านขุนกลาง</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำบ้านยาง</t>
+  </si>
+  <si>
+    <t>CLB</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนจุฬาภรณ์</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนขนาดเล็กเขื่อนห้วยกุ่ม</t>
+  </si>
+  <si>
+    <t>SCLB</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำท้ายเขื่อนจุฬาภรณ์</t>
+  </si>
+  <si>
+    <t>KKC</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนแก่งกระจาน</t>
+  </si>
+  <si>
+    <t>CHK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำคลองช่องกล่ำ</t>
+  </si>
+  <si>
+    <t>SRD</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนสิรินธร</t>
+  </si>
+  <si>
+    <t>PMN</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนปากมูล</t>
+  </si>
+  <si>
+    <t>SRK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนสิริกิติ์</t>
+  </si>
+  <si>
+    <t>NRS</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนนเรศวร</t>
+  </si>
+  <si>
+    <t>KNO</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนแควน้อยบำรุงแดน</t>
+  </si>
+  <si>
+    <t>KOT</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนคลองตรอน</t>
+  </si>
+  <si>
+    <t>PCK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนผาจุก</t>
+  </si>
+  <si>
+    <t>VRK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนวชิราลงกรณ</t>
+  </si>
+  <si>
+    <t>HKM</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำห้วยกุยมั่ง</t>
+  </si>
+  <si>
+    <t>TSK</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังงานแสงอาทิตย์ทับสะแก</t>
+  </si>
+  <si>
+    <t>RPB</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังน้ำเขื่อนรัชชประภา</t>
+  </si>
+  <si>
+    <t>PTP</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้ากังหันลมแหลมพรหมเทพ</t>
+  </si>
+  <si>
+    <t>CHILDID</t>
+  </si>
+  <si>
+    <t>worktype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +771,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -625,7 +833,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -913,9 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1263,6 +1469,622 @@
       </c>
       <c r="C31" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63907BCF-4EC9-48F4-927F-20E2C75E39F1}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20E00A5-D725-42A5-8918-7CA27021B907}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8EE3F3-C069-4512-8722-59C9FDBD6644}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1870,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A98B5FE-7DCD-4FB5-86B1-BE0833578E03}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2125,326 +2947,612 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="A32" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="A33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="A35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="A39" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="A40" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+      <c r="A41" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="A42" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="A44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+      <c r="A45" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="A47" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="A49" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
+      <c r="A51" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
+      <c r="A52" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
+      <c r="A53" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
+      <c r="A54" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
+      <c r="A55" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
+      <c r="A56" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+      <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
+      <c r="A58" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
+      <c r="A59" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
+      <c r="A60" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
+      <c r="A61" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
+      <c r="A62" t="s">
         <v>163</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="1" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB254297-F9CA-466E-8573-4D02F75784A2}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="9"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+    <sortCondition ref="A1:A34"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update and fix .html
</commit_message>
<xml_diff>
--- a/static/excel/Database.xlsx
+++ b/static/excel/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narav\Downloads\maximo\WebConverter\maximo_project\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AD65F7-F351-4A3A-9AD8-CB723A21F403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C03CF-3B41-4A22-BA69-06F750109B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="213">
   <si>
     <t>EGAT</t>
   </si>
@@ -675,6 +675,18 @@
   </si>
   <si>
     <t>SBK0</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าลำตะคองชลภาวัฒนา</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าพลังแสงทิตย์ทับสะแก</t>
+  </si>
+  <si>
+    <t>โรงไฟฟ้าดีเซลแม่ฮ่องสอน</t>
   </si>
 </sst>
 </file>
@@ -855,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -902,6 +914,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,7 +1337,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>0</v>
@@ -1635,7 +1654,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20E00A5-D725-42A5-8918-7CA27021B907}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1867,7 +1886,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1875,23 +1894,23 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1899,7 +1918,7 @@
         <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1907,7 +1926,7 @@
         <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1915,7 +1934,103 @@
         <v>115</v>
       </c>
       <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1928,7 +2043,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1769735-B55F-4AA7-B776-CD12A3415048}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,8 +2243,8 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7">
-        <v>10</v>
+      <c r="B2" s="7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2137,7 +2252,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2145,7 +2260,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2153,7 +2268,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2161,7 +2276,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2169,7 +2284,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="7">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2177,7 +2292,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2185,7 +2300,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2193,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="7">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2201,7 +2316,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2209,7 +2324,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2217,7 +2332,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="7">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2225,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="7">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2233,15 +2348,15 @@
         <v>20</v>
       </c>
       <c r="B15" s="7">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="8">
-        <v>50</v>
+      <c r="B16" s="7">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2249,7 +2364,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="8">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2257,23 +2372,23 @@
         <v>20</v>
       </c>
       <c r="B18" s="8">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="7">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="8">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7">
-        <v>11</v>
+      <c r="B20" s="7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2281,7 +2396,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2289,7 +2404,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="7">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2297,7 +2412,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2305,7 +2420,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2313,7 +2428,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2321,7 +2436,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="7">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2329,7 +2444,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="7">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2337,7 +2452,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="7">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2345,7 +2460,7 @@
         <v>23</v>
       </c>
       <c r="B29" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2353,7 +2468,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="7">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2361,7 +2476,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="7">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2369,23 +2484,23 @@
         <v>23</v>
       </c>
       <c r="B32" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="8">
-        <v>50</v>
+      <c r="B33" s="7">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="8">
-        <v>51</v>
+      <c r="B34" s="7">
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2393,31 +2508,31 @@
         <v>23</v>
       </c>
       <c r="B35" s="8">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="B36" s="8">
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
+      </c>
+      <c r="B37" s="8">
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>40</v>
+      <c r="B38" s="7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2425,7 +2540,7 @@
         <v>26</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2433,7 +2548,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2441,7 +2556,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2449,7 +2564,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2457,7 +2572,7 @@
         <v>26</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2465,31 +2580,31 @@
         <v>26</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2497,7 +2612,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2505,7 +2620,7 @@
         <v>29</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2513,7 +2628,7 @@
         <v>29</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2521,7 +2636,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2529,7 +2644,7 @@
         <v>29</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2537,39 +2652,39 @@
         <v>29</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>41</v>
+      <c r="B57" s="7" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2577,7 +2692,7 @@
         <v>31</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2585,7 +2700,7 @@
         <v>31</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -2593,7 +2708,7 @@
         <v>31</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2601,7 +2716,7 @@
         <v>31</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -2609,39 +2724,39 @@
         <v>31</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="5">
-        <v>10</v>
+      <c r="B63" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="5">
-        <v>11</v>
+      <c r="B64" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="5">
-        <v>12</v>
+      <c r="B65" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="5">
-        <v>13</v>
+      <c r="B66" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -2649,7 +2764,7 @@
         <v>31</v>
       </c>
       <c r="B67" s="5">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -2657,7 +2772,7 @@
         <v>31</v>
       </c>
       <c r="B68" s="5">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -2665,7 +2780,7 @@
         <v>31</v>
       </c>
       <c r="B69" s="5">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -2673,7 +2788,7 @@
         <v>31</v>
       </c>
       <c r="B70" s="5">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -2681,7 +2796,7 @@
         <v>31</v>
       </c>
       <c r="B71" s="5">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -2689,7 +2804,7 @@
         <v>31</v>
       </c>
       <c r="B72" s="5">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -2697,7 +2812,7 @@
         <v>31</v>
       </c>
       <c r="B73" s="5">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -2705,7 +2820,7 @@
         <v>31</v>
       </c>
       <c r="B74" s="5">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -2713,7 +2828,7 @@
         <v>31</v>
       </c>
       <c r="B75" s="5">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -2721,7 +2836,7 @@
         <v>31</v>
       </c>
       <c r="B76" s="5">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -2729,7 +2844,7 @@
         <v>31</v>
       </c>
       <c r="B77" s="5">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -2737,7 +2852,7 @@
         <v>31</v>
       </c>
       <c r="B78" s="5">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -2745,39 +2860,39 @@
         <v>31</v>
       </c>
       <c r="B79" s="5">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B80" s="5">
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="B81" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="B82" s="5">
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="B83" s="5">
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -2785,7 +2900,7 @@
         <v>115</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -2793,7 +2908,7 @@
         <v>115</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -2801,7 +2916,7 @@
         <v>115</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -2809,7 +2924,7 @@
         <v>115</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -2817,39 +2932,39 @@
         <v>115</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B89" s="5">
-        <v>10</v>
+      <c r="B89" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B90" s="5">
-        <v>11</v>
+      <c r="B90" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="5">
-        <v>12</v>
+      <c r="B91" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B92" s="5">
-        <v>13</v>
+      <c r="B92" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -2857,7 +2972,7 @@
         <v>115</v>
       </c>
       <c r="B93" s="5">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -2865,7 +2980,7 @@
         <v>115</v>
       </c>
       <c r="B94" s="5">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -2873,7 +2988,7 @@
         <v>115</v>
       </c>
       <c r="B95" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -2881,7 +2996,7 @@
         <v>115</v>
       </c>
       <c r="B96" s="5">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -2889,7 +3004,7 @@
         <v>115</v>
       </c>
       <c r="B97" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -2897,7 +3012,7 @@
         <v>115</v>
       </c>
       <c r="B98" s="5">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2905,7 +3020,7 @@
         <v>115</v>
       </c>
       <c r="B99" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2913,7 +3028,7 @@
         <v>115</v>
       </c>
       <c r="B100" s="5">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2921,7 +3036,7 @@
         <v>115</v>
       </c>
       <c r="B101" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2929,7 +3044,7 @@
         <v>115</v>
       </c>
       <c r="B102" s="5">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2937,7 +3052,7 @@
         <v>115</v>
       </c>
       <c r="B103" s="5">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2945,7 +3060,7 @@
         <v>115</v>
       </c>
       <c r="B104" s="5">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -2953,7 +3068,7 @@
         <v>115</v>
       </c>
       <c r="B105" s="5">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2961,7 +3076,7 @@
         <v>115</v>
       </c>
       <c r="B106" s="5">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2969,32 +3084,68 @@
         <v>115</v>
       </c>
       <c r="B107" s="5">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B108" s="8">
-        <v>50</v>
+      <c r="B108" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B109" s="8">
-        <v>51</v>
+      <c r="B109" s="5">
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B110" s="8">
-        <v>52</v>
-      </c>
+      <c r="B110" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B111" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="8"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="8"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3005,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB254297-F9CA-466E-8573-4D02F75784A2}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3223,7 +3374,7 @@
         <v>127</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
         <v>127</v>
@@ -3377,7 +3528,7 @@
         <v>146</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E27" t="s">
         <v>146</v>
@@ -3431,7 +3582,7 @@
         <v>158</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -5228,7 +5379,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5322,10 +5473,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9DF26F-8AEA-46DE-A532-DF9A156B3D07}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5333,168 +5484,467 @@
     <col min="1" max="1" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>31</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>52</v>
       </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D112" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix bug error mapping
</commit_message>
<xml_diff>
--- a/static/excel/Database.xlsx
+++ b/static/excel/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narav\Downloads\maximo\WebConverter\maximo_project\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C03CF-3B41-4A22-BA69-06F750109B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B09DCC-FF78-4E00-9E2D-DD61358B4FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="1" r:id="rId1"/>
@@ -867,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -914,13 +914,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +1201,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1954,7 +1950,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B37" t="s">
@@ -1962,7 +1958,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B38" t="s">
@@ -1970,7 +1966,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B39" t="s">
@@ -1978,7 +1974,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B40" t="s">
@@ -1986,7 +1982,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B41" t="s">
@@ -1994,7 +1990,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B42" t="s">
@@ -2002,7 +1998,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B43" t="s">
@@ -2010,7 +2006,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B44" t="s">
@@ -2018,7 +2014,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B45" t="s">
@@ -2026,7 +2022,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B46" t="s">
@@ -2043,7 +2039,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1769735-B55F-4AA7-B776-CD12A3415048}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3157,7 +3153,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3694,7 +3690,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4560,7 +4556,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5379,7 +5375,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5476,7 +5472,7 @@
   <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5494,7 +5490,7 @@
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="7" t="s">
         <v>209</v>
       </c>
       <c r="B2" s="28"/>
@@ -6063,7 +6059,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>